<commit_message>
Update to docker/yml files
</commit_message>
<xml_diff>
--- a/src/test/resources/data/loginTestDataPW.xlsx
+++ b/src/test/resources/data/loginTestDataPW.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D33744-4A2A-46BD-9020-D4BF59BB6935}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D627DBC3-9E1A-4A2F-9543-C7DB614EBA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validUsers" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -62,10 +62,13 @@
     <t>test@example.com</t>
   </si>
   <si>
-    <t>natePW@mailinator.com</t>
-  </si>
-  <si>
     <t>te</t>
+  </si>
+  <si>
+    <t>natashatestpw@gmail.com</t>
+  </si>
+  <si>
+    <t>3230474N5a5t5e5!</t>
   </si>
 </sst>
 </file>
@@ -399,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,10 +425,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -443,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5390205-5823-4FC1-B471-E0F6E6EB5F10}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -468,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -479,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>

</xml_diff>